<commit_message>
What is your name
</commit_message>
<xml_diff>
--- a/Unicorn/Answers/HackathonQuestionsExcel.xlsx
+++ b/Unicorn/Answers/HackathonQuestionsExcel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="97">
   <si>
     <t>What is MailboxIQ and what does it do?</t>
   </si>
@@ -296,9 +296,6 @@
     <t>How are you?</t>
   </si>
   <si>
-    <t>What's your name?</t>
-  </si>
-  <si>
     <t>What is your name?</t>
   </si>
   <si>
@@ -329,13 +326,19 @@
     <t>How are you today?</t>
   </si>
   <si>
-    <t>Yo, I'm the Banking Unicorn, hear me roar,
-In the world of finance, I'm the one they adore,
-From transactions to savings, I'm the star of the show,
-When you ask my name, now you know where I glow!</t>
-  </si>
-  <si>
     <t>Can you be trained?</t>
+  </si>
+  <si>
+    <t>Yo, I'm the Banking Unicorn, hear me roar, In the world of finance, I'm the one they adore, From transactions to savings, I'm the star of the show, When you ask my name, now you know where I glow!</t>
+  </si>
+  <si>
+    <t>Can say about the features of the app?</t>
+  </si>
+  <si>
+    <t>What are the main features of the MailBoxIQ app?</t>
+  </si>
+  <si>
+    <t>How can I start using the App?</t>
   </si>
 </sst>
 </file>
@@ -669,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -693,7 +696,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>72</v>
       </c>
@@ -704,7 +707,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>72</v>
       </c>
@@ -715,15 +718,15 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>93</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
@@ -731,7 +734,7 @@
         <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>11</v>
@@ -750,13 +753,13 @@
     </row>
     <row r="7" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
@@ -764,54 +767,54 @@
         <v>50</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="116" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="87" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
@@ -819,21 +822,21 @@
         <v>54</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>86</v>
+        <v>21</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
@@ -841,21 +844,21 @@
         <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>22</v>
+        <v>87</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
@@ -863,21 +866,21 @@
         <v>56</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>88</v>
+        <v>23</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>32</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -885,10 +888,10 @@
         <v>80</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -896,76 +899,76 @@
         <v>80</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
@@ -973,32 +976,32 @@
         <v>62</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="58" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="58" x14ac:dyDescent="0.35">
@@ -1006,32 +1009,32 @@
         <v>64</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
@@ -1039,86 +1042,108 @@
         <v>66</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="58" x14ac:dyDescent="0.35">
-      <c r="A34" s="3" t="s">
+    <row r="36" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A36" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="116" x14ac:dyDescent="0.35">
-      <c r="A35" s="3" t="s">
+    <row r="37" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="87" x14ac:dyDescent="0.35">
-      <c r="A37" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="3" t="s">
+    <row r="41" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="58" x14ac:dyDescent="0.35">
-      <c r="A40" s="3" t="s">
+    <row r="42" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A42" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>